<commit_message>
Fixed height of one cell that was off
</commit_message>
<xml_diff>
--- a/projectManagement/Gantt_Diagramm.xlsx
+++ b/projectManagement/Gantt_Diagramm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NightPic\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="11_3512C0102C17460564B422FE575E14EA12868D28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D49EB0F-AD12-42D0-88B6-1DE963B2C17A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Diagramm" sheetId="1" r:id="rId1"/>
@@ -122,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -257,18 +256,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -284,9 +271,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,19 +621,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="22" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="2" max="3" width="22.75" customWidth="1"/>
+    <col min="4" max="22" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="54">
@@ -647,55 +646,55 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="19" t="s">
+      <c r="F2" s="15"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="19"/>
+      <c r="J2" s="15"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="19"/>
+      <c r="N2" s="15"/>
       <c r="P2" s="8"/>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="19"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="39.950000000000003" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:19" ht="15.95" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="3">
         <v>1</v>
       </c>
@@ -779,13 +778,13 @@
       <c r="C6" s="7">
         <v>3</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="H6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="N6" s="15"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="H6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="P6" s="4"/>
       <c r="R6" s="4"/>
     </row>
@@ -802,10 +801,10 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="H7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="N7" s="15"/>
+      <c r="H7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="P7" s="4"/>
       <c r="R7" s="4"/>
     </row>
@@ -822,15 +821,15 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="H8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="N8" s="15"/>
+      <c r="H8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="N8" s="11"/>
       <c r="P8" s="4"/>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:19" ht="30" customHeight="1">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="7">
@@ -850,7 +849,7 @@
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:19" ht="30" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7">
@@ -861,22 +860,22 @@
       </c>
       <c r="D10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
       <c r="J10" s="4"/>
       <c r="L10" s="4"/>
       <c r="N10" s="4"/>
       <c r="P10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:19" ht="30.75">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:19" ht="28.5" customHeight="1">
+      <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="14">
         <v>4</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="14">
         <v>2</v>
       </c>
       <c r="D11" s="4"/>
@@ -909,7 +908,7 @@
       <c r="P12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:19" ht="30.75">
+    <row r="13" spans="1:19" ht="30">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -943,9 +942,9 @@
       <c r="D14" s="4"/>
       <c r="F14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="4"/>
       <c r="N14" s="4"/>
       <c r="P14" s="4"/>
@@ -993,13 +992,13 @@
       <c r="R16" s="4"/>
     </row>
     <row r="17" spans="1:18" ht="30" customHeight="1">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="14">
         <v>10</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="14">
         <v>2</v>
       </c>
       <c r="D17" s="4"/>
@@ -1013,33 +1012,33 @@
       <c r="R17" s="4"/>
     </row>
     <row r="18" spans="1:18" ht="30" customHeight="1">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="14">
         <v>9</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="14">
         <v>2</v>
       </c>
       <c r="D18" s="4"/>
       <c r="F18" s="4"/>
       <c r="H18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
       <c r="N18" s="4"/>
       <c r="P18" s="4"/>
       <c r="R18" s="4"/>
     </row>
     <row r="19" spans="1:18" ht="30" customHeight="1">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="14">
         <v>9</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="14">
         <v>2</v>
       </c>
       <c r="D19" s="4"/>
@@ -1074,13 +1073,13 @@
       <c r="R20" s="4"/>
     </row>
     <row r="21" spans="1:18" ht="30" customHeight="1">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="14">
         <v>12</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="14">
         <v>1</v>
       </c>
       <c r="D21" s="4"/>
@@ -1094,13 +1093,13 @@
       <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:18" ht="30" customHeight="1">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="14">
         <v>11</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="14">
         <v>2</v>
       </c>
       <c r="D22" s="4"/>
@@ -1108,19 +1107,19 @@
       <c r="H22" s="4"/>
       <c r="J22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4"/>
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18" ht="30" customHeight="1">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="14">
         <v>12</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="14">
         <v>1</v>
       </c>
       <c r="D23" s="4"/>
@@ -1153,13 +1152,13 @@
       <c r="R24" s="4"/>
     </row>
     <row r="25" spans="1:18" ht="30" customHeight="1">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="14">
         <v>13</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="14">
         <v>2</v>
       </c>
       <c r="D25" s="4"/>
@@ -1172,13 +1171,13 @@
       <c r="R25" s="4"/>
     </row>
     <row r="26" spans="1:18" ht="30" customHeight="1">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="14">
         <v>13</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="14">
         <v>1</v>
       </c>
       <c r="D26" s="4"/>
@@ -1187,18 +1186,18 @@
       <c r="J26" s="4"/>
       <c r="L26" s="4"/>
       <c r="N26" s="4"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
       <c r="R26" s="4"/>
     </row>
     <row r="27" spans="1:18" ht="30" customHeight="1">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="14">
         <v>12</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="14">
         <v>1</v>
       </c>
       <c r="D27" s="4"/>
@@ -1350,11 +1349,6 @@
       <c r="P40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="42" spans="4:18" ht="15"/>
-    <row r="43" spans="4:18" ht="15"/>
-    <row r="44" spans="4:18" ht="15"/>
-    <row r="45" spans="4:18" ht="15"/>
-    <row r="46" spans="4:18" ht="15"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="E2:F2"/>

</xml_diff>

<commit_message>
Adjusted Gantt diagram and added PDF
</commit_message>
<xml_diff>
--- a/projectManagement/Gantt_Diagramm.xlsx
+++ b/projectManagement/Gantt_Diagramm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NightPic\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50F65520-4A1E-449D-B07D-76C882972282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Diagramm" sheetId="1" r:id="rId1"/>
@@ -40,16 +41,16 @@
     <t>Gantt Diagramm</t>
   </si>
   <si>
-    <t>Leon</t>
-  </si>
-  <si>
-    <t>Marco</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Marcel</t>
+    <t>Leon Kranner</t>
+  </si>
+  <si>
+    <t>Marco Kuner</t>
+  </si>
+  <si>
+    <t>David Vollmer</t>
+  </si>
+  <si>
+    <t>Marcel Wagner</t>
   </si>
   <si>
     <t>AKTIVITÄT</t>
@@ -61,7 +62,7 @@
     <t>DAUER DES PLANS</t>
   </si>
   <si>
-    <t>Zeiträume</t>
+    <t>Kalenderwoche</t>
   </si>
   <si>
     <t>Planung und Konzeption des Projektes</t>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -269,7 +270,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,7 +286,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -621,19 +622,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.75" customWidth="1"/>
-    <col min="2" max="3" width="22.75" customWidth="1"/>
-    <col min="4" max="22" width="4.75" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="22" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="54">
@@ -696,52 +697,52 @@
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I4" s="3">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="J4" s="3">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="K4" s="3">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="L4" s="3">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="M4" s="3">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="N4" s="3">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="O4" s="3">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="P4" s="3">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="Q4" s="3">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="R4" s="3">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="S4" s="3">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" customHeight="1">
@@ -1350,11 +1351,7 @@
       <c r="R40" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="Q2:R2"/>
+  <mergeCells count="4">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:O3"/>
     <mergeCell ref="B3:B4"/>

</xml_diff>